<commit_message>
Update report and readme
</commit_message>
<xml_diff>
--- a/Report/UserMapping.xlsx
+++ b/Report/UserMapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E2864-3690-4BD6-9C1C-D94494F25823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7736F1-3BD4-4A5D-B0B3-0CCCF8B30958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
   <si>
     <t>Major Features</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Make transactions</t>
   </si>
   <si>
-    <t>Input post id</t>
-  </si>
-  <si>
     <t>Feedback</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
   </si>
   <si>
     <t>UC18</t>
-  </si>
-  <si>
-    <t>UC19</t>
   </si>
   <si>
     <t>Log in with Google</t>
@@ -378,7 +372,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,13 +419,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -559,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -581,20 +568,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -622,18 +607,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -643,19 +616,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW45"/>
+  <dimension ref="A1:AW44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ33" sqref="AJ33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL20" sqref="AL20:AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,174 +920,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
     </row>
     <row r="2" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="N2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="AA2" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="AB2" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AC2" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AE2" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AF2" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AG2" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="AF2" s="11" t="s">
+      <c r="AH2" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="AG2" s="11" t="s">
+      <c r="AI2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AK2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AL2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AK2" s="11" t="s">
+      <c r="AM2" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM2" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="37"/>
+        <v>48</v>
+      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1133,7 +1101,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="37"/>
+      <c r="P3" s="31"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
@@ -1160,9 +1128,9 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="37"/>
+        <v>49</v>
+      </c>
+      <c r="B4" s="16"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1176,7 +1144,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="37"/>
+      <c r="P4" s="31"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -1203,9 +1171,9 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="B5" s="16"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1219,7 +1187,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -1246,7 +1214,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -1263,7 +1231,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="2"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1289,7 +1257,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1306,7 +1274,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="32"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1332,7 +1300,7 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1375,7 +1343,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1418,7 +1386,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1449,8 +1417,8 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
@@ -1461,7 +1429,7 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1504,7 +1472,7 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1535,9 +1503,9 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="2"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
@@ -1547,7 +1515,7 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1580,8 +1548,8 @@
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="2"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
@@ -1590,14 +1558,14 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1607,7 +1575,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="Q14" s="2"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -1624,7 +1592,7 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
-      <c r="AH14" s="2"/>
+      <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
@@ -1633,15 +1601,15 @@
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1676,7 +1644,7 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1684,8 +1652,8 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1693,10 +1661,10 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
@@ -1719,7 +1687,7 @@
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1728,8 +1696,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1737,10 +1705,10 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="2"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1762,7 +1730,7 @@
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1772,8 +1740,8 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1783,13 +1751,13 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="2"/>
+      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
@@ -1805,7 +1773,7 @@
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1816,8 +1784,8 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1831,8 +1799,8 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
@@ -1841,14 +1809,14 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
       <c r="AL19" s="3"/>
       <c r="AM19" s="3"/>
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1860,8 +1828,8 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="2"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -1884,207 +1852,164 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
-      <c r="AJ20" s="2"/>
-      <c r="AK20" s="2"/>
-      <c r="AL20" s="3"/>
-      <c r="AM20" s="3"/>
-    </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="2"/>
-      <c r="AM21" s="2"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="36"/>
-      <c r="AB22" s="36"/>
-      <c r="AC22" s="36"/>
-      <c r="AD22" s="36"/>
-      <c r="AE22" s="36"/>
-      <c r="AF22" s="36"/>
-      <c r="AG22" s="36"/>
-      <c r="AH22" s="36"/>
-      <c r="AI22" s="36"/>
-      <c r="AJ22" s="36"/>
-      <c r="AK22" s="36"/>
-      <c r="AL22" s="36"/>
-      <c r="AM22" s="36"/>
-      <c r="AQ22" s="36"/>
-      <c r="AR22" s="36"/>
-      <c r="AS22" s="36"/>
-      <c r="AT22" s="36"/>
-      <c r="AU22" s="36"/>
-      <c r="AV22" s="36"/>
-      <c r="AW22" s="36"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="15"/>
+      <c r="AL22" s="15"/>
+      <c r="AM22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+      <c r="AS22" s="15"/>
+      <c r="AT22" s="15"/>
+      <c r="AU22" s="15"/>
+      <c r="AV22" s="15"/>
+      <c r="AW22" s="15"/>
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
-      <c r="AA23" s="36"/>
-      <c r="AB23" s="36"/>
-      <c r="AC23" s="36"/>
-      <c r="AD23" s="36"/>
-      <c r="AE23" s="36"/>
-      <c r="AF23" s="36"/>
-      <c r="AG23" s="36"/>
-      <c r="AH23" s="36"/>
-      <c r="AI23" s="36"/>
-      <c r="AJ23" s="36"/>
-      <c r="AK23" s="36"/>
-      <c r="AL23" s="36"/>
-      <c r="AM23" s="36"/>
-      <c r="AN23" s="36"/>
-      <c r="AO23" s="36"/>
-      <c r="AP23" s="36"/>
-      <c r="AQ23" s="36"/>
-      <c r="AR23" s="36"/>
-      <c r="AS23" s="36"/>
-      <c r="AT23" s="36"/>
-      <c r="AU23" s="36"/>
-      <c r="AV23" s="36"/>
-      <c r="AW23" s="36"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="15"/>
+      <c r="AJ23" s="15"/>
+      <c r="AK23" s="15"/>
+      <c r="AL23" s="15"/>
+      <c r="AM23" s="15"/>
+      <c r="AN23" s="15"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+      <c r="AR23" s="15"/>
+      <c r="AS23" s="15"/>
+      <c r="AT23" s="15"/>
+      <c r="AU23" s="15"/>
+      <c r="AV23" s="15"/>
+      <c r="AW23" s="15"/>
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="36"/>
-      <c r="AC24" s="36"/>
-      <c r="AD24" s="36"/>
-      <c r="AE24" s="36"/>
-      <c r="AF24" s="36"/>
-      <c r="AG24" s="36"/>
-      <c r="AH24" s="36"/>
-      <c r="AI24" s="36"/>
-      <c r="AJ24" s="36"/>
-      <c r="AK24" s="36"/>
-      <c r="AL24" s="36"/>
-      <c r="AM24" s="36"/>
-      <c r="AN24" s="36"/>
-      <c r="AO24" s="36"/>
-      <c r="AP24" s="36"/>
-      <c r="AQ24" s="36"/>
-      <c r="AR24" s="36"/>
-      <c r="AS24" s="36"/>
-      <c r="AT24" s="36"/>
-      <c r="AU24" s="36"/>
-      <c r="AV24" s="36"/>
-      <c r="AW24" s="36"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="15"/>
+      <c r="AT24" s="15"/>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="15"/>
+      <c r="AW24" s="15"/>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B26" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -2100,7 +2025,7 @@
       <c r="M26" s="21"/>
       <c r="N26" s="22"/>
       <c r="P26" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q26" s="21"/>
       <c r="R26" s="21"/>
@@ -2110,7 +2035,7 @@
       <c r="V26" s="22"/>
       <c r="W26" s="9"/>
       <c r="X26" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y26" s="21"/>
       <c r="Z26" s="21"/>
@@ -2123,10 +2048,10 @@
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -2134,10 +2059,10 @@
       <c r="G27" s="25"/>
       <c r="H27" s="4"/>
       <c r="I27" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
@@ -2145,10 +2070,10 @@
       <c r="N27" s="25"/>
       <c r="O27" s="4"/>
       <c r="P27" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q27" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R27" s="24"/>
       <c r="S27" s="24"/>
@@ -2157,10 +2082,10 @@
       <c r="V27" s="25"/>
       <c r="W27" s="9"/>
       <c r="X27" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y27" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z27" s="24"/>
       <c r="AA27" s="24"/>
@@ -2172,10 +2097,10 @@
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -2183,10 +2108,10 @@
       <c r="G28" s="25"/>
       <c r="H28" s="4"/>
       <c r="I28" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
@@ -2194,10 +2119,10 @@
       <c r="N28" s="25"/>
       <c r="O28" s="4"/>
       <c r="P28" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R28" s="24"/>
       <c r="S28" s="24"/>
@@ -2206,10 +2131,10 @@
       <c r="V28" s="25"/>
       <c r="W28" s="9"/>
       <c r="X28" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Y28" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z28" s="24"/>
       <c r="AA28" s="24"/>
@@ -2221,10 +2146,10 @@
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -2232,10 +2157,10 @@
       <c r="G29" s="25"/>
       <c r="H29" s="4"/>
       <c r="I29" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
@@ -2243,10 +2168,10 @@
       <c r="N29" s="25"/>
       <c r="O29" s="4"/>
       <c r="P29" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q29" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R29" s="24"/>
       <c r="S29" s="24"/>
@@ -2255,10 +2180,10 @@
       <c r="V29" s="25"/>
       <c r="W29" s="9"/>
       <c r="X29" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Y29" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z29" s="18"/>
       <c r="AA29" s="18"/>
@@ -2270,7 +2195,7 @@
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>3</v>
@@ -2281,10 +2206,10 @@
       <c r="G30" s="25"/>
       <c r="H30" s="4"/>
       <c r="I30" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
@@ -2292,10 +2217,10 @@
       <c r="N30" s="25"/>
       <c r="O30" s="4"/>
       <c r="P30" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q30" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R30" s="24"/>
       <c r="S30" s="24"/>
@@ -2304,10 +2229,10 @@
       <c r="V30" s="25"/>
       <c r="W30" s="9"/>
       <c r="X30" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Y30" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
@@ -2319,7 +2244,7 @@
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>11</v>
@@ -2330,10 +2255,10 @@
       <c r="G31" s="25"/>
       <c r="H31" s="4"/>
       <c r="I31" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
@@ -2341,10 +2266,10 @@
       <c r="N31" s="25"/>
       <c r="O31" s="4"/>
       <c r="P31" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
@@ -2353,10 +2278,10 @@
       <c r="V31" s="25"/>
       <c r="W31" s="9"/>
       <c r="X31" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Y31" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z31" s="18"/>
       <c r="AA31" s="18"/>
@@ -2368,7 +2293,7 @@
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>12</v>
@@ -2379,10 +2304,10 @@
       <c r="G32" s="25"/>
       <c r="H32" s="4"/>
       <c r="I32" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
@@ -2390,10 +2315,10 @@
       <c r="N32" s="25"/>
       <c r="O32" s="4"/>
       <c r="P32" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R32" s="24"/>
       <c r="S32" s="24"/>
@@ -2402,10 +2327,10 @@
       <c r="V32" s="25"/>
       <c r="W32" s="9"/>
       <c r="X32" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Y32" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z32" s="18"/>
       <c r="AA32" s="18"/>
@@ -2417,7 +2342,7 @@
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>8</v>
@@ -2428,10 +2353,10 @@
       <c r="G33" s="25"/>
       <c r="H33" s="4"/>
       <c r="I33" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
@@ -2439,10 +2364,10 @@
       <c r="N33" s="25"/>
       <c r="O33" s="4"/>
       <c r="P33" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q33" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R33" s="24"/>
       <c r="S33" s="24"/>
@@ -2451,10 +2376,10 @@
       <c r="V33" s="25"/>
       <c r="W33" s="9"/>
       <c r="X33" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Y33" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z33" s="18"/>
       <c r="AA33" s="18"/>
@@ -2466,7 +2391,7 @@
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>13</v>
@@ -2477,21 +2402,21 @@
       <c r="G34" s="25"/>
       <c r="H34" s="4"/>
       <c r="I34" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J34" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="35"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="28"/>
       <c r="O34" s="4"/>
       <c r="P34" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q34" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R34" s="24"/>
       <c r="S34" s="24"/>
@@ -2500,10 +2425,10 @@
       <c r="V34" s="25"/>
       <c r="W34" s="9"/>
       <c r="X34" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Y34" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z34" s="18"/>
       <c r="AA34" s="18"/>
@@ -2515,10 +2440,10 @@
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -2526,21 +2451,21 @@
       <c r="G35" s="25"/>
       <c r="H35" s="4"/>
       <c r="I35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="32"/>
+        <v>80</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="14"/>
       <c r="O35" s="4"/>
       <c r="P35" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q35" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R35" s="24"/>
       <c r="S35" s="24"/>
@@ -2549,10 +2474,10 @@
       <c r="V35" s="25"/>
       <c r="W35" s="9"/>
       <c r="X35" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Y35" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
@@ -2564,7 +2489,7 @@
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>14</v>
@@ -2575,21 +2500,21 @@
       <c r="G36" s="25"/>
       <c r="H36" s="4"/>
       <c r="I36" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J36" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="35"/>
+        <v>81</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="28"/>
       <c r="O36" s="4"/>
       <c r="P36" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q36" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R36" s="24"/>
       <c r="S36" s="24"/>
@@ -2598,10 +2523,10 @@
       <c r="V36" s="25"/>
       <c r="W36" s="9"/>
       <c r="X36" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y36" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z36" s="18"/>
       <c r="AA36" s="18"/>
@@ -2613,7 +2538,7 @@
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>15</v>
@@ -2624,21 +2549,21 @@
       <c r="G37" s="25"/>
       <c r="H37" s="4"/>
       <c r="I37" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="J37" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="35"/>
+        <v>82</v>
+      </c>
+      <c r="J37" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="28"/>
       <c r="O37" s="4"/>
       <c r="P37" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q37" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R37" s="24"/>
       <c r="S37" s="24"/>
@@ -2647,10 +2572,10 @@
       <c r="V37" s="25"/>
       <c r="W37" s="9"/>
       <c r="X37" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Y37" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Z37" s="18"/>
       <c r="AA37" s="18"/>
@@ -2662,10 +2587,10 @@
     </row>
     <row r="38" spans="2:32" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -2673,10 +2598,10 @@
       <c r="G38" s="25"/>
       <c r="H38" s="4"/>
       <c r="I38" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
@@ -2684,10 +2609,10 @@
       <c r="N38" s="25"/>
       <c r="O38" s="4"/>
       <c r="P38" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q38" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R38" s="24"/>
       <c r="S38" s="24"/>
@@ -2696,10 +2621,10 @@
       <c r="V38" s="25"/>
       <c r="W38" s="9"/>
       <c r="X38" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Y38" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z38" s="18"/>
       <c r="AA38" s="18"/>
@@ -2711,10 +2636,10 @@
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -2723,10 +2648,10 @@
       <c r="H39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q39" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R39" s="24"/>
       <c r="S39" s="24"/>
@@ -2735,10 +2660,10 @@
       <c r="V39" s="25"/>
       <c r="W39" s="9"/>
       <c r="X39" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Y39" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z39" s="18"/>
       <c r="AA39" s="18"/>
@@ -2750,10 +2675,10 @@
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
@@ -2779,16 +2704,16 @@
       <c r="AF40" s="9"/>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B41" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
+      <c r="B41" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="19"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -2817,15 +2742,15 @@
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="19"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2847,15 +2772,15 @@
     </row>
     <row r="43" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="19"/>
       <c r="W43" s="9"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="9"/>
@@ -2869,50 +2794,37 @@
     </row>
     <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="16"/>
-    </row>
-    <row r="45" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B45" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="62">
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="R1:AM1"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="Q29:V29"/>
+    <mergeCell ref="Y29:AF29"/>
+    <mergeCell ref="Y28:AF28"/>
     <mergeCell ref="Y27:AF27"/>
     <mergeCell ref="Q28:V28"/>
     <mergeCell ref="Q27:V27"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="C27:G27"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="R1:AM1"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C39:G39"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="C33:G33"/>
     <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
     <mergeCell ref="C40:G40"/>
     <mergeCell ref="J27:N27"/>
     <mergeCell ref="J28:N28"/>
@@ -2925,8 +2837,10 @@
     <mergeCell ref="J36:N36"/>
     <mergeCell ref="J37:N37"/>
     <mergeCell ref="J38:N38"/>
-    <mergeCell ref="Q29:V29"/>
-    <mergeCell ref="Y31:AF31"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
     <mergeCell ref="Q30:V30"/>
     <mergeCell ref="Q31:V31"/>
     <mergeCell ref="Q32:V32"/>
@@ -2934,13 +2848,6 @@
     <mergeCell ref="Y32:AF32"/>
     <mergeCell ref="Y33:AF33"/>
     <mergeCell ref="Y30:AF30"/>
-    <mergeCell ref="Q34:V34"/>
-    <mergeCell ref="Q35:V35"/>
-    <mergeCell ref="Q36:V36"/>
-    <mergeCell ref="Q37:V37"/>
-    <mergeCell ref="Q38:V38"/>
-    <mergeCell ref="Y29:AF29"/>
-    <mergeCell ref="Y28:AF28"/>
     <mergeCell ref="Y39:AF39"/>
     <mergeCell ref="I26:N26"/>
     <mergeCell ref="P26:V26"/>
@@ -2951,6 +2858,16 @@
     <mergeCell ref="Y37:AF37"/>
     <mergeCell ref="Y38:AF38"/>
     <mergeCell ref="Q39:V39"/>
+    <mergeCell ref="Q34:V34"/>
+    <mergeCell ref="Q35:V35"/>
+    <mergeCell ref="Q36:V36"/>
+    <mergeCell ref="Q37:V37"/>
+    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="Y31:AF31"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>